<commit_message>
update projection of prediction layers
</commit_message>
<xml_diff>
--- a/04_Modelling/01_benthic/01_BRUVs/BRT_Output_bruvs/contrib_mod_best_fixed_Log_biomass_gaussian.xlsx
+++ b/04_Modelling/01_benthic/01_BRUVs/BRT_Output_bruvs/contrib_mod_best_fixed_Log_biomass_gaussian.xlsx
@@ -376,7 +376,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>57.47241449087687</v>
+        <v>57.71561539619783</v>
       </c>
     </row>
     <row r="3">
@@ -386,7 +386,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>10.52522096529903</v>
+        <v>10.75824539048188</v>
       </c>
     </row>
     <row r="4">
@@ -396,7 +396,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>10.01854719107467</v>
+        <v>10.05735555675508</v>
       </c>
     </row>
     <row r="5">
@@ -406,7 +406,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>8.525680212277901</v>
+        <v>8.701212397762976</v>
       </c>
     </row>
     <row r="6">
@@ -416,7 +416,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>6.939699607027515</v>
+        <v>6.738617788281282</v>
       </c>
     </row>
     <row r="7">
@@ -426,7 +426,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>6.518437533444024</v>
+        <v>6.02895347052096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>